<commit_message>
refs #848 Gewichtung begründet
Former-commit-id: 3e533796cb65cf1579bd7ba322ac6ba659cb3b39
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/06_Entwurf/NutzwertanalyseAuswahlKinectSDK.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/06_Entwurf/NutzwertanalyseAuswahlKinectSDK.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -88,7 +88,7 @@
     <t>Durch die Nutzwertanalyse geht das "Framework 1: Kinect for Windows SDK" als Sieger hervor.</t>
   </si>
   <si>
-    <t>Bemerkung: Die Gewichtungs- / Bewertungsskala geht von 1 (am schlechtesten) bis 5 (am besten).</t>
+    <t>Bemerkung: Die Gewichtungs- / Bewertungsskala geht von wenig (1), mittel (3) bis zu sehr wichtig (5).</t>
   </si>
 </sst>
 </file>
@@ -212,6 +212,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -228,16 +238,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,48 +554,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="11"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -604,22 +604,22 @@
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -630,24 +630,24 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="16">
-        <v>5</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C5" s="10">
+        <v>5</v>
+      </c>
+      <c r="D5" s="11">
         <f>B5*C5</f>
         <v>25</v>
       </c>
-      <c r="E5" s="16">
-        <v>3</v>
-      </c>
-      <c r="F5" s="17">
+      <c r="E5" s="10">
+        <v>3</v>
+      </c>
+      <c r="F5" s="11">
         <f>B5*E5</f>
         <v>15</v>
       </c>
-      <c r="G5" s="16">
-        <v>3</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="G5" s="10">
+        <v>3</v>
+      </c>
+      <c r="H5" s="11">
         <f>B5*G5</f>
         <v>15</v>
       </c>
@@ -659,24 +659,24 @@
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="16">
-        <v>5</v>
-      </c>
-      <c r="D6" s="17">
+      <c r="C6" s="10">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11">
         <f>B6*C6</f>
         <v>15</v>
       </c>
-      <c r="E6" s="16">
-        <v>3</v>
-      </c>
-      <c r="F6" s="17">
+      <c r="E6" s="10">
+        <v>3</v>
+      </c>
+      <c r="F6" s="11">
         <f>B6*E6</f>
         <v>9</v>
       </c>
-      <c r="G6" s="16">
-        <v>3</v>
-      </c>
-      <c r="H6" s="17">
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="11">
         <f>B6*G6</f>
         <v>9</v>
       </c>
@@ -688,24 +688,24 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="17">
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
         <f>B7*C7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="16">
-        <v>5</v>
-      </c>
-      <c r="F7" s="17">
+      <c r="E7" s="10">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11">
         <f>B7*E7</f>
         <v>5</v>
       </c>
-      <c r="G7" s="16">
-        <v>5</v>
-      </c>
-      <c r="H7" s="17">
+      <c r="G7" s="10">
+        <v>5</v>
+      </c>
+      <c r="H7" s="11">
         <f>B7*G7</f>
         <v>5</v>
       </c>
@@ -717,24 +717,24 @@
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="16">
-        <v>5</v>
-      </c>
-      <c r="D8" s="17">
+      <c r="C8" s="10">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11">
         <f>B8*C8</f>
         <v>25</v>
       </c>
-      <c r="E8" s="16">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17">
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="11">
         <f>B8*E8</f>
         <v>15</v>
       </c>
-      <c r="G8" s="16">
-        <v>1</v>
-      </c>
-      <c r="H8" s="17">
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
         <f>B8*G8</f>
         <v>5</v>
       </c>
@@ -746,24 +746,24 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="16">
-        <v>5</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="C9" s="10">
+        <v>5</v>
+      </c>
+      <c r="D9" s="11">
         <f t="shared" ref="D9:D14" si="0">B9*C9</f>
         <v>25</v>
       </c>
-      <c r="E9" s="16">
-        <v>3</v>
-      </c>
-      <c r="F9" s="17">
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
+      <c r="F9" s="11">
         <f t="shared" ref="F9:F14" si="1">B9*E9</f>
         <v>15</v>
       </c>
-      <c r="G9" s="16">
-        <v>1</v>
-      </c>
-      <c r="H9" s="17">
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
         <f t="shared" ref="H9:H14" si="2">B9*G9</f>
         <v>5</v>
       </c>
@@ -775,24 +775,24 @@
       <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="C10" s="16">
-        <v>3</v>
-      </c>
-      <c r="D10" s="17">
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E10" s="16">
-        <v>5</v>
-      </c>
-      <c r="F10" s="17">
+      <c r="E10" s="10">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G10" s="16">
-        <v>1</v>
-      </c>
-      <c r="H10" s="17">
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -804,24 +804,24 @@
       <c r="B11" s="5">
         <v>5</v>
       </c>
-      <c r="C11" s="16">
-        <v>3</v>
-      </c>
-      <c r="D11" s="17">
+      <c r="C11" s="10">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E11" s="16">
-        <v>5</v>
-      </c>
-      <c r="F11" s="17">
+      <c r="E11" s="10">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="G11" s="16">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -833,24 +833,24 @@
       <c r="B12" s="5">
         <v>5</v>
       </c>
-      <c r="C12" s="16">
-        <v>5</v>
-      </c>
-      <c r="D12" s="17">
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E12" s="16">
-        <v>3</v>
-      </c>
-      <c r="F12" s="17">
+      <c r="E12" s="10">
+        <v>3</v>
+      </c>
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G12" s="16">
-        <v>1</v>
-      </c>
-      <c r="H12" s="17">
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -862,24 +862,24 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17">
+      <c r="C13" s="10">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E13" s="16">
-        <v>5</v>
-      </c>
-      <c r="F13" s="17">
+      <c r="E13" s="10">
+        <v>5</v>
+      </c>
+      <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G13" s="16">
-        <v>5</v>
-      </c>
-      <c r="H13" s="17">
+      <c r="G13" s="10">
+        <v>5</v>
+      </c>
+      <c r="H13" s="11">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -891,24 +891,24 @@
       <c r="B14" s="5">
         <v>3</v>
       </c>
-      <c r="C14" s="16">
-        <v>5</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="C14" s="10">
+        <v>5</v>
+      </c>
+      <c r="D14" s="11">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="17">
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G14" s="16">
-        <v>1</v>
-      </c>
-      <c r="H14" s="17">
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -918,18 +918,18 @@
         <v>5</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19">
+      <c r="C15" s="12"/>
+      <c r="D15" s="13">
         <f>SUM(D5:D14)</f>
         <v>158</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19">
+      <c r="E15" s="12"/>
+      <c r="F15" s="13">
         <f>SUM(F5:F14)</f>
         <v>132</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19">
+      <c r="G15" s="12"/>
+      <c r="H15" s="13">
         <f>SUM(H5:H14)</f>
         <v>70</v>
       </c>
@@ -939,46 +939,46 @@
         <v>4</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13">
         <f>IF(D15&gt;=F15,IF(D15&gt;=H15,1,2),IF(D15&gt;=H15,2,3))</f>
         <v>1</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19">
+      <c r="E16" s="12"/>
+      <c r="F16" s="13">
         <f>IF(F15&gt;=H15,IF(F15&gt;=D15,1,2),IF(F15&gt;=D15,2,3))</f>
         <v>2</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19">
+      <c r="G16" s="12"/>
+      <c r="H16" s="13">
         <f>IF(H15&gt;=D15,IF(H15&gt;=F15,1,2),IF(H15&gt;=F15,2,3))</f>
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>